<commit_message>
uff... load on postgresql complete, created a copuple of reports and a view to get rapid insight on ufxm2
</commit_message>
<xml_diff>
--- a/excel/HouseMarket.xlsx
+++ b/excel/HouseMarket.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Reference\housemodel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Reference\housemodel\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D80F816-FFDC-4964-B5A6-10912BFB6E33}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0450CA68-D482-4328-BBC6-FA6F6C007A48}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2070" yWindow="2070" windowWidth="9600" windowHeight="6600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Segments" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="10">
   <si>
     <t>Segment 1</t>
   </si>
@@ -46,6 +46,15 @@
   </si>
   <si>
     <t>Bdroom</t>
+  </si>
+  <si>
+    <t>Segment fullScan</t>
+  </si>
+  <si>
+    <t>Region</t>
+  </si>
+  <si>
+    <t>RM</t>
   </si>
 </sst>
 </file>
@@ -147,7 +156,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -158,6 +167,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -440,10 +452,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -499,9 +511,62 @@
       </c>
       <c r="C5" s="1"/>
     </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="1">
+        <v>1000</v>
+      </c>
+      <c r="C9" s="1">
+        <v>25000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="1"/>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A7:C7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>